<commit_message>
new db v 0.8
</commit_message>
<xml_diff>
--- a/data_call/415061327.xlsx
+++ b/data_call/415061327.xlsx
@@ -344,7 +344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -897,6 +897,24 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>501+ ЛЕНТА МАСКИР. ОДНОСТ., ОСНОВА БУМ., АДГЕЗИВ КАУЧУК., БЕЖ.; 0048 ММХ 0055,0 М</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>нескладской / срок поставки 62 дн.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>